<commit_message>
H & M Modified The Transactions & The Excel Identity Mapping sheets respectivly
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_ExcelPayIdentity.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_ExcelPayIdentity.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cold LKPs" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="AspNetRoles" sheetId="7" r:id="rId2"/>
     <sheet name="AspNetUsers" sheetId="1" r:id="rId3"/>
     <sheet name="AspNetUserRoles" sheetId="3" r:id="rId4"/>
     <sheet name="AspNetUserClaims" sheetId="4" r:id="rId5"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
   <si>
     <t>TRGT_Columns</t>
   </si>
@@ -121,61 +121,16 @@
     <t xml:space="preserve">  FROM [ExcelpayIdentity_Stage].[dbo].[AspNetUserClaims]</t>
   </si>
   <si>
-    <t>users</t>
-  </si>
-  <si>
-    <t>permissions</t>
-  </si>
-  <si>
-    <t>roles</t>
-  </si>
-  <si>
-    <t>AspNetUserClaims</t>
-  </si>
-  <si>
-    <t>AspNetUserRoles</t>
-  </si>
-  <si>
-    <t>AspNetUserLogins</t>
-  </si>
-  <si>
     <t>AspNetUsers</t>
   </si>
   <si>
     <t>model_has_roles</t>
   </si>
   <si>
-    <t>AspNetUserTokens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ,[email]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ,[phone]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ,[password]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ,[created_at]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ,[updated_at]</t>
-  </si>
-  <si>
-    <t>role_id</t>
-  </si>
-  <si>
-    <t>model_id</t>
-  </si>
-  <si>
     <t>ثابته من عبد الناصر</t>
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>واحده من عندهم ع الكل</t>
   </si>
   <si>
     <t>null</t>
@@ -195,17 +150,116 @@
     <t>fk roles</t>
   </si>
   <si>
-    <t>unique identified</t>
-  </si>
-  <si>
-    <t>Users</t>
+    <t>[id]</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>[name]</t>
+  </si>
+  <si>
+    <t>[email]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [bigint]</t>
+  </si>
+  <si>
+    <t>[created_at]</t>
+  </si>
+  <si>
+    <t>[phone]</t>
+  </si>
+  <si>
+    <t>[password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [datetime]</t>
+  </si>
+  <si>
+    <t>[updated_at]</t>
+  </si>
+  <si>
+    <t>[nvarchar](20)</t>
+  </si>
+  <si>
+    <t>[nvarchar](50)</t>
+  </si>
+  <si>
+    <t>[nvarchar](191)</t>
+  </si>
+  <si>
+    <t>[dbo].[Users]</t>
+  </si>
+  <si>
+    <t>Calculated using some Logic (Update Statements)</t>
+  </si>
+  <si>
+    <t>Calculated Column</t>
+  </si>
+  <si>
+    <t>Auto Generated</t>
+  </si>
+  <si>
+    <t>one to one</t>
+  </si>
+  <si>
+    <t>Brought from another Table</t>
+  </si>
+  <si>
+    <t>[Name]</t>
+  </si>
+  <si>
+    <t>[NormalizedName]</t>
+  </si>
+  <si>
+    <t>[dbo].[Roles]</t>
+  </si>
+  <si>
+    <t>[numeric](20, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [nvarchar](191)</t>
+  </si>
+  <si>
+    <t>[datetime]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[id] </t>
+  </si>
+  <si>
+    <t>[guard_name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[created_at] </t>
+  </si>
+  <si>
+    <t>[model_type]</t>
+  </si>
+  <si>
+    <t>[model_id]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[role_id] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[numeric](20, 0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'JBLJTPJFIIDIFTV2RJ44LV3B2BHN3FIY'</t>
+  </si>
+  <si>
+    <t>'985ba9aa-5a7d-4c39-9584-b6e3b21e7760'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[nvarchar](191) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,13 +283,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,11 +342,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -537,41 +635,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -581,64 +663,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:E7"/>
+  <dimension ref="D2:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D1" t="s">
+    <row r="2" spans="4:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>33</v>
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -648,32 +797,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:L23"/>
+  <dimension ref="D3:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:12" s="1" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="4:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
@@ -687,47 +838,63 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E5" s="3" t="s">
-        <v>53</v>
+    <row r="5" spans="4:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
       </c>
       <c r="K5" t="s">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="K6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="K8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H9">
         <v>0</v>
       </c>
@@ -735,39 +902,63 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="K10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="K11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="K12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H14">
         <v>0</v>
       </c>
@@ -775,42 +966,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>50</v>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>73</v>
       </c>
       <c r="K16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>50</v>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>74</v>
       </c>
       <c r="K17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>0</v>
       </c>
@@ -818,7 +1018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>0</v>
       </c>
@@ -826,7 +1026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>0</v>
       </c>
@@ -834,7 +1034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>0</v>
       </c>
@@ -842,12 +1042,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F23" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="K23" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F26" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F27" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -858,27 +1081,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:M6"/>
+  <dimension ref="E1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:13" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2" t="s">
         <v>21</v>
@@ -894,29 +1123,94 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>46</v>
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="M6" t="s">
+    </row>
+    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="3" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -926,22 +1220,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:M9"/>
+  <dimension ref="E1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="55" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:13" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
@@ -964,7 +1257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
         <v>31</v>
       </c>
@@ -972,25 +1265,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H- Fixed Some Stuff regarding The Identity and added the identitiy to TRGT Package
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_ExcelPayIdentity.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_To_Excel_Mapping_Sheet_ExcelPayIdentity.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cold LKPs" sheetId="2" r:id="rId1"/>
-    <sheet name="AspNetRoles" sheetId="7" r:id="rId2"/>
-    <sheet name="AspNetUsers" sheetId="1" r:id="rId3"/>
-    <sheet name="AspNetUserRoles" sheetId="3" r:id="rId4"/>
-    <sheet name="AspNetUserClaims" sheetId="4" r:id="rId5"/>
+    <sheet name="AspNetUsers" sheetId="1" r:id="rId2"/>
+    <sheet name="AspNetUserRoles" sheetId="8" r:id="rId3"/>
+    <sheet name="AspNetUserClaims" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>TRGT_Columns</t>
   </si>
@@ -125,9 +124,6 @@
   </si>
   <si>
     <t>model_has_roles</t>
-  </si>
-  <si>
-    <t>ثابته من عبد الناصر</t>
   </si>
   <si>
     <t>name</t>
@@ -156,9 +152,6 @@
     <t>Data type</t>
   </si>
   <si>
-    <t>[name]</t>
-  </si>
-  <si>
     <t>[email]</t>
   </si>
   <si>
@@ -207,39 +200,9 @@
     <t>Brought from another Table</t>
   </si>
   <si>
-    <t>[Name]</t>
-  </si>
-  <si>
-    <t>[NormalizedName]</t>
-  </si>
-  <si>
-    <t>[dbo].[Roles]</t>
-  </si>
-  <si>
-    <t>[numeric](20, 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [nvarchar](191)</t>
-  </si>
-  <si>
-    <t>[datetime]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[id] </t>
-  </si>
-  <si>
-    <t>[guard_name]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[created_at] </t>
-  </si>
-  <si>
     <t>[model_type]</t>
   </si>
   <si>
-    <t>[model_id]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[role_id] </t>
   </si>
   <si>
@@ -252,14 +215,44 @@
     <t>'985ba9aa-5a7d-4c39-9584-b6e3b21e7760'</t>
   </si>
   <si>
-    <t xml:space="preserve">[nvarchar](191) </t>
+    <t>auto_Generated</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>[ExcelpayIdentity_Stage].[dbo].[AspNetUserClaims]</t>
+  </si>
+  <si>
+    <t>memberrole</t>
+  </si>
+  <si>
+    <t>MerchantCode</t>
+  </si>
+  <si>
+    <t>MerchantId</t>
+  </si>
+  <si>
+    <t>IsMaster</t>
+  </si>
+  <si>
+    <t>Merchantname</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>[Name,MemberRole,MerchantCode,MerchantId,IsMaster]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [nvarchar](191) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +283,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -342,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -355,6 +355,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +648,7 @@
   <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,144 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:L18"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F15" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F16" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +699,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -840,16 +716,16 @@
     </row>
     <row r="5" spans="4:12" ht="75" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
         <v>32</v>
@@ -860,13 +736,13 @@
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K6" t="s">
         <v>3</v>
@@ -874,7 +750,7 @@
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s">
         <v>4</v>
@@ -882,13 +758,13 @@
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
         <v>5</v>
@@ -904,13 +780,13 @@
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
         <v>7</v>
@@ -918,13 +794,13 @@
     </row>
     <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
         <v>8</v>
@@ -932,13 +808,13 @@
     </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K12" t="s">
         <v>9</v>
@@ -946,13 +822,13 @@
     </row>
     <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
@@ -968,13 +844,13 @@
     </row>
     <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15" t="s">
         <v>12</v>
@@ -982,7 +858,7 @@
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="K16" t="s">
         <v>13</v>
@@ -990,7 +866,7 @@
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K17" t="s">
         <v>14</v>
@@ -998,13 +874,13 @@
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
@@ -1044,7 +920,7 @@
     </row>
     <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1055,22 +931,22 @@
     </row>
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F25" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F26" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F27" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1079,138 +955,112 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:M22"/>
+  <dimension ref="F3:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E1" s="1" t="s">
+    <row r="3" spans="6:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="F3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2" t="s">
+      <c r="H3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N3" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="5:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+    <row r="5" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="G5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="3" t="s">
+    <row r="16" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="5" t="s">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="6" t="s">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="19" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1218,18 +1068,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:M18"/>
+  <dimension ref="E1:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:M1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="55" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1257,7 +1109,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="I6" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="K6" t="s">
         <v>31</v>
       </c>
@@ -1266,21 +1121,42 @@
       </c>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="L7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="L9" t="s">
         <v>28</v>
@@ -1288,27 +1164,67 @@
     </row>
     <row r="14" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="8" t="s">
-        <v>59</v>
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>